<commit_message>
Add comprehensive documentation, examples, and configuration details for Excel2Yaml
</commit_message>
<xml_diff>
--- a/HockeyRosters.xlsx
+++ b/HockeyRosters.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Excel2Yaml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{615AFA87-9B7B-41F9-817A-7977D8B172F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F835345-5ED6-4012-8DD4-0721CBA075E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{91321BCD-DCC9-4880-9BE1-BFDF087B55B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Output" sheetId="3" r:id="rId2"/>
+    <sheet name="HOCKEY_0" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
+    <sheet name="Output" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="52">
   <si>
     <t>League</t>
   </si>
@@ -187,76 +188,54 @@
         players:
           - name: Sanheim, Travis
             position: D
-            letter: A
           - name: Drysdale, Jamie
             position: D
-            letter: 
       - line: 2
         players:
           - name: York, Cam
             position: D
-            letter: 
           - name: Seeler, Nick
             position: D
-            letter: 
       - line: 3
         players:
           - name: Zamula, Egor
             position: D
-            letter: 
           - name: Andrae, Emil
             position: D
-            letter: 
-      - line: 4
-        players: []
     offense:
       - line: 1
         players:
           - name: Michkov, Matvei
             position: W
-            letter: 
           - name: Konecny, Travis
             position: W
-            letter: A
       - line: 2
         players:
           - name: Foerster, Tyson
             position: W
-            letter: 
           - name: Brink, Bobby
             position: W
-            letter: 
           - name: Tippet, Owen
             position: W
-            letter: 
       - line: 3
         players:
           - name: Pelletier, Jakob
             position: W
-            letter: 
       - line: 4
         players:
           - name: Deslauriers, Nicolas
             position: W
-            letter: 
           - name: Hathaway, Garnet
             position: W
-            letter: 
     goaltender:
       - line: 1
         players:
           - name: Ersson, Samuel
             position: G
-            letter: 
       - line: 2
         players:
           - name: Fedotov, Ivan
             position: G
-            letter: 
-      - line: 3
-        players: []
-      - line: 4
-        players: []
 ---
 # AHL
 team:
@@ -276,49 +255,60 @@
         players:
           - name: Andrae, Emil
             position: D
-            letter: A
       - line: 2
         players:
           - name: Belpedio, Louie
             position: D
-            letter: 
       - line: 3
         players:
           - name: Hogberg, Linus
             position: D
-            letter: 
     offense:
       - line: 1
         players:
           - name: Wilson, Garrett
             position: W
-            letter: C
           - name: Lycksell, Olle
             position: W
-            letter: A
           - name: Anisimov, Artem
             position: W
-            letter: 
       - line: 2
         players:
           - name: Wisdom, Zayde
             position: W
-            letter: 
-      - line: 3
-        players: []
     goaltender:
       - line: 1
         players:
           - name: Gahagen, Parker
             position: G
-            letter: 
       - line: 2
         players:
           - name: Sandstrom, Felix
-            position: G
-            letter: 
-      - line: 3
-        players: []</t>
+            position: G</t>
+  </si>
+  <si>
+    <t>Provorov, Ivan</t>
+  </si>
+  <si>
+    <t>Farabee, Joel</t>
+  </si>
+  <si>
+    <t>Hart, Carter</t>
+  </si>
+  <si>
+    <t>Penguins</t>
+  </si>
+  <si>
+    <t>Crosby, Sidney</t>
+  </si>
+  <si>
+    <t>Guentzel, Jake</t>
+  </si>
+  <si>
+    <t>Letang, Kris</t>
+  </si>
+  <si>
+    <t>Jarry, Tristan</t>
   </si>
 </sst>
 </file>
@@ -381,15 +371,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>115956</xdr:colOff>
+      <xdr:colOff>480391</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>770282</xdr:rowOff>
+      <xdr:rowOff>654326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>903356</xdr:colOff>
+      <xdr:colOff>1267791</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1062382</xdr:rowOff>
+      <xdr:rowOff>946426</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -407,7 +397,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2269434" y="770282"/>
+          <a:off x="2633869" y="654326"/>
           <a:ext cx="787400" cy="292100"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -472,6 +462,21 @@
     <tableColumn id="6" xr3:uid="{99910525-0732-423E-BC8F-0723C475923B}" name="Letter"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D5AB0E2-2560-4EBC-82A3-7F13F57649EA}" name="Table3" displayName="Table3" ref="B2:G14" totalsRowShown="0">
+  <autoFilter ref="B2:G14" xr:uid="{7D5AB0E2-2560-4EBC-82A3-7F13F57649EA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E130878E-F560-4F01-93A1-5B144AA1D0B9}" name="League"/>
+    <tableColumn id="2" xr3:uid="{5CEE1231-89BC-4B14-9BAF-5474497158D9}" name="Team"/>
+    <tableColumn id="3" xr3:uid="{9611ADB6-C234-453E-BA68-3A0D2B804A36}" name="Position"/>
+    <tableColumn id="4" xr3:uid="{21C57DF4-A709-408A-8219-B099B74B72FC}" name="Player"/>
+    <tableColumn id="5" xr3:uid="{5658E3EB-2B9F-4A4E-B033-11D7C5F5D238}" name="Line"/>
+    <tableColumn id="6" xr3:uid="{873715BA-6B5F-44B6-8293-D3B59CE2BADA}" name="Letter"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -795,8 +800,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,11 +1361,276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4895BA76-455A-4FA4-A714-1A7DD033AC75}">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708EED82-BBEA-4D25-84F5-867C20EAC883}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>